<commit_message>
admittance matrix measurement added
</commit_message>
<xml_diff>
--- a/Merilna oprema.xlsx
+++ b/Merilna oprema.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unilj-my.sharepoint.com/personal/vrtac_fs1_uni-lj_si/Documents/Documents/Doktorat/Projekt_1/Faza V - nova struktura/Eksperiment/Impact testing v2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unilj-my.sharepoint.com/personal/vrtac_fs1_uni-lj_si/Documents/Documents/Doktorat/Python_scripts/Impact testing v2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="8_{D8C0E4B4-90D8-440C-A191-4C23A391F473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C8F31F1-2346-4A69-BC75-E9E23898E247}"/>
+  <xr:revisionPtr revIDLastSave="107" documentId="8_{D8C0E4B4-90D8-440C-A191-4C23A391F473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BCAF0F1-D406-474E-A3E5-A7F4952F8773}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BA12A476-02EB-496D-9FD7-3A34AAF1406E}"/>
+    <workbookView xWindow="98895" yWindow="0" windowWidth="12810" windowHeight="15135" xr2:uid="{BA12A476-02EB-496D-9FD7-3A34AAF1406E}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="47">
   <si>
     <t>Model</t>
   </si>
@@ -164,10 +164,19 @@
     <t>45250</t>
   </si>
   <si>
-    <t>084A14</t>
-  </si>
-  <si>
     <t>34788</t>
+  </si>
+  <si>
+    <t>T333B30</t>
+  </si>
+  <si>
+    <t>53360</t>
+  </si>
+  <si>
+    <t>359598</t>
+  </si>
+  <si>
+    <t>LW164400</t>
   </si>
 </sst>
 </file>
@@ -617,10 +626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACB995EC-0121-456F-A805-EABFC5775035}">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,11 +713,11 @@
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>7</v>
@@ -1685,10 +1694,10 @@
       <c r="E33" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F33">
-        <v>-45</v>
-      </c>
-      <c r="G33">
+      <c r="F33" s="8">
+        <v>-45</v>
+      </c>
+      <c r="G33" s="8">
         <v>45</v>
       </c>
       <c r="H33" s="8" t="s">
@@ -1698,6 +1707,230 @@
         <v>98.74</v>
       </c>
       <c r="J33" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F34" s="8">
+        <v>-45</v>
+      </c>
+      <c r="G34" s="8">
+        <v>45</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I34" s="8">
+        <v>100.5</v>
+      </c>
+      <c r="J34" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F35" s="4">
+        <v>-45</v>
+      </c>
+      <c r="G35" s="4">
+        <v>45</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I35" s="4">
+        <v>102.5</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" t="s">
+        <v>18</v>
+      </c>
+      <c r="F36">
+        <v>-45</v>
+      </c>
+      <c r="G36">
+        <v>45</v>
+      </c>
+      <c r="H36" t="s">
+        <v>38</v>
+      </c>
+      <c r="I36">
+        <v>101.4</v>
+      </c>
+      <c r="J36" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F37" s="8">
+        <v>-45</v>
+      </c>
+      <c r="G37" s="8">
+        <v>45</v>
+      </c>
+      <c r="H37" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I37" s="8">
+        <v>99.5</v>
+      </c>
+      <c r="J37" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D38" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" t="s">
+        <v>16</v>
+      </c>
+      <c r="F38">
+        <v>-45</v>
+      </c>
+      <c r="G38">
+        <v>45</v>
+      </c>
+      <c r="H38" t="s">
+        <v>38</v>
+      </c>
+      <c r="I38">
+        <v>97.95</v>
+      </c>
+      <c r="J38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D39" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" t="s">
+        <v>18</v>
+      </c>
+      <c r="F39">
+        <v>-45</v>
+      </c>
+      <c r="G39">
+        <v>45</v>
+      </c>
+      <c r="H39" t="s">
+        <v>38</v>
+      </c>
+      <c r="I39">
+        <v>100.21</v>
+      </c>
+      <c r="J39" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F40" s="8">
+        <v>-45</v>
+      </c>
+      <c r="G40" s="8">
+        <v>45</v>
+      </c>
+      <c r="H40" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I40" s="8">
+        <v>99.81</v>
+      </c>
+      <c r="J40" s="8" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>